<commit_message>
update summary bill for stage 01
</commit_message>
<xml_diff>
--- a/bills/summary.xlsx
+++ b/bills/summary.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PCB\Altium Designer\Temperature_station_DMAn\envIoT\bills\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google_Drive\3.Projects\envIoT\bills\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0877BAD-10BD-4100-816E-EC232421BC61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>STT</t>
   </si>
@@ -65,9 +66,6 @@
     <t>phí vận chuyển hàng lên SG</t>
   </si>
   <si>
-    <t>Tổng</t>
-  </si>
-  <si>
     <t>Thanh toán</t>
   </si>
   <si>
@@ -77,16 +75,25 @@
     <t>Phích cắm điện</t>
   </si>
   <si>
-    <t>Đơn mua lẻ ở An Lạc</t>
-  </si>
-  <si>
     <t>Tâm</t>
+  </si>
+  <si>
+    <t>Đơn mua lẻ ở An Lạc + test oscil</t>
+  </si>
+  <si>
+    <t>An+Tâm</t>
+  </si>
+  <si>
+    <t>Thực tổng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tổng </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$VND]\ #,##0"/>
   </numFmts>
@@ -452,22 +459,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="33" customWidth="1"/>
-    <col min="4" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="4" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -487,10 +494,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -512,10 +519,10 @@
         <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -534,10 +541,10 @@
       </c>
       <c r="F3" s="4"/>
       <c r="G3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -559,10 +566,10 @@
         <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -581,10 +588,10 @@
       </c>
       <c r="F5" s="4"/>
       <c r="G5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -603,30 +610,32 @@
       </c>
       <c r="F6" s="2"/>
       <c r="G6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2">
-        <v>2</v>
-      </c>
-      <c r="D7" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="D7" s="3">
+        <v>12000</v>
+      </c>
       <c r="E7" s="3">
         <f>C7*D7</f>
-        <v>0</v>
+        <v>36000</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -637,18 +646,18 @@
         <v>1</v>
       </c>
       <c r="D8" s="3">
-        <v>120000</v>
+        <v>150000</v>
       </c>
       <c r="E8" s="3">
         <f t="shared" ref="E8" si="2">C8*D8</f>
-        <v>120000</v>
+        <v>150000</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -656,86 +665,97 @@
       <c r="E9" s="3"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="3">
         <f>SUM(E2:E9)</f>
-        <v>2237950</v>
+        <v>2303950</v>
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="1">
+        <v>1800000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E12" s="1">
+        <f>E11-E10</f>
+        <v>-503950</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:D11"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F4" r:id="rId2"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>